<commit_message>
added additional analysis and planned comparison F-test ananlysis
</commit_message>
<xml_diff>
--- a/Data/Intersubject Correlations.xlsx
+++ b/Data/Intersubject Correlations.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erezfreud/Documents/Shape_Sensitivity_LifeSpan/Analyzed/Shape_Sensetivity_LifeSpan/voxel_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Jenn\Documents\ShapeSensitivity\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053FD377-0AE3-4D12-90EF-23433F470EF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="32">
   <si>
     <t>VR</t>
   </si>
@@ -106,11 +115,29 @@
   <si>
     <t>Novel Ventral Intersubject Correlations (Fisher Transformed)</t>
   </si>
+  <si>
+    <t>Interobject intersubject Correlations (Raw)</t>
+  </si>
+  <si>
+    <t>S vs. N - Ventral</t>
+  </si>
+  <si>
+    <t>S vs. N - Dorsal</t>
+  </si>
+  <si>
+    <t>N vs. S Ventral</t>
+  </si>
+  <si>
+    <t>N vs. S Dorsal</t>
+  </si>
+  <si>
+    <t>Interobject intersubject Correlations (Fisher Transformed)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -140,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -148,6 +175,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,6 +188,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -424,74 +458,83 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AG64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AI23" sqref="AI23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="5" max="6" width="11.5" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="15" max="15" width="13.6640625" customWidth="1"/>
-    <col min="16" max="16" width="14.6640625" customWidth="1"/>
-    <col min="17" max="17" width="13.1640625" customWidth="1"/>
-    <col min="22" max="22" width="22.83203125" customWidth="1"/>
-    <col min="25" max="25" width="15.33203125" customWidth="1"/>
-    <col min="26" max="26" width="13.1640625" customWidth="1"/>
-    <col min="27" max="27" width="15.5" customWidth="1"/>
-    <col min="30" max="30" width="13.33203125" customWidth="1"/>
-    <col min="31" max="32" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="22" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="33" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
       <c r="M1" s="1"/>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
       <c r="X1" s="1"/>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
       <c r="AC1" s="1"/>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="2"/>
-      <c r="AG1" s="2"/>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -583,7 +626,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -675,7 +718,7 @@
         <v>0.59296187682840495</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -767,7 +810,7 @@
         <v>0.73559525266191395</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -859,7 +902,7 @@
         <v>0.71210894107303002</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -951,7 +994,7 @@
         <v>0.22302619420741901</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1043,7 +1086,7 @@
         <v>0.53057017057400802</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1135,7 +1178,7 @@
         <v>0.71437525418241199</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1227,7 +1270,7 @@
         <v>0.646785883961284</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1319,7 +1362,7 @@
         <v>0.70073288687588298</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1411,7 +1454,7 @@
         <v>0.76510064933588295</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1503,7 +1546,7 @@
         <v>0.61528179577757702</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1595,7 +1638,7 @@
         <v>0.77989820980102698</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1687,7 +1730,7 @@
         <v>0.68933376953742698</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -1803,51 +1846,51 @@
         <v>0.64214757373468911</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B17" s="2" t="s">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="2" t="s">
+      <c r="N17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
       <c r="R17" s="1"/>
-      <c r="S17" s="2" t="s">
+      <c r="S17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
       <c r="X17" s="1"/>
-      <c r="Y17" s="2" t="s">
+      <c r="Y17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z17" s="2"/>
-      <c r="AA17" s="2"/>
-      <c r="AB17" s="2"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
+      <c r="AB17" s="3"/>
       <c r="AC17" s="1"/>
-      <c r="AD17" s="2" t="s">
+      <c r="AD17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AE17" s="2"/>
-      <c r="AF17" s="2"/>
-      <c r="AG17" s="2"/>
-    </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="3"/>
+      <c r="AG17" s="3"/>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
@@ -1939,24 +1982,24 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1</v>
       </c>
       <c r="B19">
-        <f>FISHER(B3)</f>
+        <f t="shared" ref="B19:E30" si="10">FISHER(B3)</f>
         <v>1.1461816262803808</v>
       </c>
       <c r="C19">
-        <f>FISHER(C3)</f>
+        <f t="shared" si="10"/>
         <v>1.0924504160648583</v>
       </c>
       <c r="D19">
-        <f>FISHER(D3)</f>
+        <f t="shared" si="10"/>
         <v>0.88319899742500907</v>
       </c>
       <c r="E19">
-        <f>FISHER(E3)</f>
+        <f t="shared" si="10"/>
         <v>0.78659476745865442</v>
       </c>
       <c r="G19" s="1">
@@ -1967,15 +2010,15 @@
         <v>1.0923679557718158</v>
       </c>
       <c r="I19">
-        <f t="shared" ref="I19:K19" si="10">FISHER(I3)</f>
+        <f t="shared" ref="I19:K19" si="11">FISHER(I3)</f>
         <v>0.98254460774439034</v>
       </c>
       <c r="J19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.83737492685322157</v>
       </c>
       <c r="K19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.79032950355042486</v>
       </c>
       <c r="M19" s="1">
@@ -1986,15 +2029,15 @@
         <v>0.97361850198762867</v>
       </c>
       <c r="O19">
-        <f t="shared" ref="O19:Q19" si="11">FISHER(O3)</f>
+        <f t="shared" ref="O19:Q19" si="12">FISHER(O3)</f>
         <v>0.5866397640560691</v>
       </c>
       <c r="P19">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.75528639908181439</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.60656978449477539</v>
       </c>
       <c r="R19" s="1">
@@ -2005,15 +2048,15 @@
         <v>1.3436429042034777</v>
       </c>
       <c r="T19">
-        <f t="shared" ref="T19:V19" si="12">FISHER(T3)</f>
+        <f t="shared" ref="T19:V19" si="13">FISHER(T3)</f>
         <v>0.56466682996754947</v>
       </c>
       <c r="U19">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1.399450942342984</v>
       </c>
       <c r="V19">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.83419369870909266</v>
       </c>
       <c r="X19" s="1">
@@ -2024,15 +2067,15 @@
         <v>0.87441059033437307</v>
       </c>
       <c r="Z19">
-        <f t="shared" ref="Z19:AB19" si="13">FISHER(Z3)</f>
+        <f t="shared" ref="Z19:AB19" si="14">FISHER(Z3)</f>
         <v>0.68113074423309805</v>
       </c>
       <c r="AA19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.94883622627887831</v>
       </c>
       <c r="AB19">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.70266432291754599</v>
       </c>
       <c r="AC19" s="1">
@@ -2043,1295 +2086,1295 @@
         <v>1.3150581737596836</v>
       </c>
       <c r="AE19">
-        <f t="shared" ref="AE19:AG19" si="14">FISHER(AE3)</f>
+        <f t="shared" ref="AE19:AG19" si="15">FISHER(AE3)</f>
         <v>0.60188765618120887</v>
       </c>
       <c r="AF19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.3567196494641951</v>
       </c>
       <c r="AG19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.682221764079044</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2</v>
       </c>
       <c r="B20">
-        <f>FISHER(B4)</f>
+        <f t="shared" si="10"/>
         <v>1.3321372086390553</v>
       </c>
       <c r="C20">
-        <f>FISHER(C4)</f>
+        <f t="shared" si="10"/>
         <v>1.2814049316478386</v>
       </c>
       <c r="D20">
-        <f>FISHER(D4)</f>
+        <f t="shared" si="10"/>
         <v>0.64927727926655676</v>
       </c>
       <c r="E20">
-        <f>FISHER(E4)</f>
+        <f t="shared" si="10"/>
         <v>0.45696673725285186</v>
       </c>
       <c r="G20" s="1">
         <v>2</v>
       </c>
       <c r="H20">
-        <f t="shared" ref="H20:K30" si="15">FISHER(H4)</f>
+        <f t="shared" ref="H20:K30" si="16">FISHER(H4)</f>
         <v>1.1080885977433852</v>
       </c>
       <c r="I20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.089994113246648</v>
       </c>
       <c r="J20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.3462091584175595</v>
       </c>
       <c r="K20">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.66120222076668234</v>
       </c>
       <c r="M20" s="1">
         <v>2</v>
       </c>
       <c r="N20">
-        <f t="shared" ref="N20:Q30" si="16">FISHER(N4)</f>
+        <f t="shared" ref="N20:Q30" si="17">FISHER(N4)</f>
         <v>0.76144459888594895</v>
       </c>
       <c r="O20">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.39985152591284473</v>
       </c>
       <c r="P20">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.72124358690331902</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>8.3371140509016783E-2</v>
       </c>
       <c r="R20" s="1">
         <v>2</v>
       </c>
       <c r="S20">
-        <f t="shared" ref="S20:V30" si="17">FISHER(S4)</f>
+        <f t="shared" ref="S20:V30" si="18">FISHER(S4)</f>
         <v>1.4691348240114803</v>
       </c>
       <c r="T20">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.78177293686508542</v>
       </c>
       <c r="U20">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.4097925485567888</v>
       </c>
       <c r="V20">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.82655005751832411</v>
       </c>
       <c r="X20" s="1">
         <v>2</v>
       </c>
       <c r="Y20">
-        <f t="shared" ref="Y20:AB20" si="18">FISHER(Y4)</f>
+        <f t="shared" ref="Y20:AB20" si="19">FISHER(Y4)</f>
         <v>0.53438835299433052</v>
       </c>
       <c r="Z20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.42060616734260414</v>
       </c>
       <c r="AA20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.86449362648962202</v>
       </c>
       <c r="AB20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.42985493689960413</v>
       </c>
       <c r="AC20" s="1">
         <v>2</v>
       </c>
       <c r="AD20">
-        <f t="shared" ref="AD20:AG20" si="19">FISHER(AD4)</f>
+        <f t="shared" ref="AD20:AG20" si="20">FISHER(AD4)</f>
         <v>1.5032589971228056</v>
       </c>
       <c r="AE20">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1.0564513732686971</v>
       </c>
       <c r="AF20">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1.5809016725360485</v>
       </c>
       <c r="AG20">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.94081232784781532</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>3</v>
       </c>
       <c r="B21">
-        <f>FISHER(B5)</f>
+        <f t="shared" si="10"/>
         <v>1.0303439598921769</v>
       </c>
       <c r="C21">
-        <f>FISHER(C5)</f>
+        <f t="shared" si="10"/>
         <v>1.214900113369856</v>
       </c>
       <c r="D21">
-        <f>FISHER(D5)</f>
+        <f t="shared" si="10"/>
         <v>1.088954158878856</v>
       </c>
       <c r="E21">
-        <f>FISHER(E5)</f>
+        <f t="shared" si="10"/>
         <v>0.82617367501586736</v>
       </c>
       <c r="G21" s="1">
         <v>3</v>
       </c>
       <c r="H21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.0694197132766046</v>
       </c>
       <c r="I21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.009282613612092</v>
       </c>
       <c r="J21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.61142176218053235</v>
       </c>
       <c r="K21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.60000711609296931</v>
       </c>
       <c r="M21" s="1">
         <v>3</v>
       </c>
       <c r="N21">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.66600233121071961</v>
       </c>
       <c r="O21">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.77845609457216824</v>
       </c>
       <c r="P21">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.6327023532490117</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.0012770004035756</v>
       </c>
       <c r="R21" s="1">
         <v>3</v>
       </c>
       <c r="S21">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.1424234178164843</v>
       </c>
       <c r="T21">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.77023095576792622</v>
       </c>
       <c r="U21">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.1454667818661965</v>
       </c>
       <c r="V21">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.90980612736522193</v>
       </c>
       <c r="X21" s="1">
         <v>3</v>
       </c>
       <c r="Y21">
-        <f t="shared" ref="Y21:AB21" si="20">FISHER(Y5)</f>
+        <f t="shared" ref="Y21:AB21" si="21">FISHER(Y5)</f>
         <v>1.1760895551173804</v>
       </c>
       <c r="Z21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.58185243359011696</v>
       </c>
       <c r="AA21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1.287612568099471</v>
       </c>
       <c r="AB21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.78252628293648518</v>
       </c>
       <c r="AC21" s="1">
         <v>3</v>
       </c>
       <c r="AD21">
-        <f t="shared" ref="AD21:AG21" si="21">FISHER(AD5)</f>
+        <f t="shared" ref="AD21:AG21" si="22">FISHER(AD5)</f>
         <v>1.2980570404937581</v>
       </c>
       <c r="AE21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.8114667817868737</v>
       </c>
       <c r="AF21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.98015901857659671</v>
       </c>
       <c r="AG21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.89144952376073261</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>4</v>
       </c>
       <c r="B22">
-        <f>FISHER(B6)</f>
+        <f t="shared" si="10"/>
         <v>0.85341358040295001</v>
       </c>
       <c r="C22">
-        <f>FISHER(C6)</f>
+        <f t="shared" si="10"/>
         <v>0.76656007645731639</v>
       </c>
       <c r="D22">
-        <f>FISHER(D6)</f>
+        <f t="shared" si="10"/>
         <v>0.83493257980866065</v>
       </c>
       <c r="E22">
-        <f>FISHER(E6)</f>
+        <f t="shared" si="10"/>
         <v>0.21884332169775478</v>
       </c>
       <c r="G22" s="1">
         <v>4</v>
       </c>
       <c r="H22">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.62022381777974178</v>
       </c>
       <c r="I22">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.69580035857893308</v>
       </c>
       <c r="J22">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.79691233221996494</v>
       </c>
       <c r="K22">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.34935989379361332</v>
       </c>
       <c r="M22" s="1">
         <v>4</v>
       </c>
       <c r="N22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.16554695145160148</v>
       </c>
       <c r="O22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.4434593941466658</v>
       </c>
       <c r="P22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.67551660990286178</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.62916324779274901</v>
       </c>
       <c r="R22" s="1">
         <v>4</v>
       </c>
       <c r="S22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.88806826502267378</v>
       </c>
       <c r="T22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.54464712956008188</v>
       </c>
       <c r="U22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.0794471532748839</v>
       </c>
       <c r="V22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.3370973399621302</v>
       </c>
       <c r="X22" s="1">
         <v>4</v>
       </c>
       <c r="Y22">
-        <f t="shared" ref="Y22:AB22" si="22">FISHER(Y6)</f>
+        <f t="shared" ref="Y22:AB22" si="23">FISHER(Y6)</f>
         <v>0.29462441909757436</v>
       </c>
       <c r="Z22">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>-2.2017703264014806E-2</v>
       </c>
       <c r="AA22">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1.0224305079860803</v>
       </c>
       <c r="AB22">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.31648840324571575</v>
       </c>
       <c r="AC22" s="1">
         <v>4</v>
       </c>
       <c r="AD22">
-        <f t="shared" ref="AD22:AG22" si="23">FISHER(AD6)</f>
+        <f t="shared" ref="AD22:AG22" si="24">FISHER(AD6)</f>
         <v>1.0392934845151431</v>
       </c>
       <c r="AE22">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.18101753821988398</v>
       </c>
       <c r="AF22">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1.4677049466049588</v>
       </c>
       <c r="AG22">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.22683845781585182</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>5</v>
       </c>
       <c r="B23">
-        <f>FISHER(B7)</f>
+        <f t="shared" si="10"/>
         <v>0.82361989943819547</v>
       </c>
       <c r="C23">
-        <f>FISHER(C7)</f>
+        <f t="shared" si="10"/>
         <v>0.94656703350035154</v>
       </c>
       <c r="D23">
-        <f>FISHER(D7)</f>
+        <f t="shared" si="10"/>
         <v>0.7208543955737291</v>
       </c>
       <c r="E23">
-        <f>FISHER(E7)</f>
+        <f t="shared" si="10"/>
         <v>0.68019955989453218</v>
       </c>
       <c r="G23" s="1">
         <v>5</v>
       </c>
       <c r="H23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.79843343475000561</v>
       </c>
       <c r="I23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.8349414595866147</v>
       </c>
       <c r="J23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.87052161961599595</v>
       </c>
       <c r="K23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.78260219264630593</v>
       </c>
       <c r="M23" s="1">
         <v>5</v>
       </c>
       <c r="N23">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.675582327349738</v>
       </c>
       <c r="O23">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.57283948790742856</v>
       </c>
       <c r="P23">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.71871831496391614</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.74418673565923621</v>
       </c>
       <c r="R23" s="1">
         <v>5</v>
       </c>
       <c r="S23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.91846866216843293</v>
       </c>
       <c r="T23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.67246951391025267</v>
       </c>
       <c r="U23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.1677720432420995</v>
       </c>
       <c r="V23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.67030902563947814</v>
       </c>
       <c r="X23" s="1">
         <v>5</v>
       </c>
       <c r="Y23">
-        <f t="shared" ref="Y23:AB23" si="24">FISHER(Y7)</f>
+        <f t="shared" ref="Y23:AB23" si="25">FISHER(Y7)</f>
         <v>0.78293079188937409</v>
       </c>
       <c r="Z23">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.3045611612165805</v>
       </c>
       <c r="AA23">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.71825246424008626</v>
       </c>
       <c r="AB23">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0.68425927247296703</v>
       </c>
       <c r="AC23" s="1">
         <v>5</v>
       </c>
       <c r="AD23">
-        <f t="shared" ref="AD23:AG23" si="25">FISHER(AD7)</f>
+        <f t="shared" ref="AD23:AG23" si="26">FISHER(AD7)</f>
         <v>1.0091452635646028</v>
       </c>
       <c r="AE23">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.62493367087133322</v>
       </c>
       <c r="AF23">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1.1778702205700438</v>
       </c>
       <c r="AG23">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.59093838804247434</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>6</v>
       </c>
       <c r="B24">
-        <f>FISHER(B8)</f>
+        <f t="shared" si="10"/>
         <v>1.1557172206240653</v>
       </c>
       <c r="C24">
-        <f>FISHER(C8)</f>
+        <f t="shared" si="10"/>
         <v>1.0550845367165047</v>
       </c>
       <c r="D24">
-        <f>FISHER(D8)</f>
+        <f t="shared" si="10"/>
         <v>0.65626442584533951</v>
       </c>
       <c r="E24">
-        <f>FISHER(E8)</f>
+        <f t="shared" si="10"/>
         <v>0.32203035705137473</v>
       </c>
       <c r="G24" s="1">
         <v>6</v>
       </c>
       <c r="H24">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.0619436739113941</v>
       </c>
       <c r="I24">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.2753926417008192</v>
       </c>
       <c r="J24">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.0233170691164204</v>
       </c>
       <c r="K24">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.79170219469946645</v>
       </c>
       <c r="M24" s="1">
         <v>6</v>
       </c>
       <c r="N24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.75392780842785989</v>
       </c>
       <c r="O24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.71978116302720652</v>
       </c>
       <c r="P24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.90077176853113694</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.96259630144195585</v>
       </c>
       <c r="R24" s="1">
         <v>6</v>
       </c>
       <c r="S24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.5274039414946381</v>
       </c>
       <c r="T24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.0101174929311709</v>
       </c>
       <c r="U24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.1796686653959232</v>
       </c>
       <c r="V24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.89786905829131125</v>
       </c>
       <c r="X24" s="1">
         <v>6</v>
       </c>
       <c r="Y24">
-        <f t="shared" ref="Y24:AB24" si="26">FISHER(Y8)</f>
+        <f t="shared" ref="Y24:AB24" si="27">FISHER(Y8)</f>
         <v>0.47316380326182705</v>
       </c>
       <c r="Z24">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.22357389101740616</v>
       </c>
       <c r="AA24">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.62141664756390225</v>
       </c>
       <c r="AB24">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.75360836059122915</v>
       </c>
       <c r="AC24" s="1">
         <v>6</v>
       </c>
       <c r="AD24">
-        <f t="shared" ref="AD24:AG24" si="27">FISHER(AD8)</f>
+        <f t="shared" ref="AD24:AG24" si="28">FISHER(AD8)</f>
         <v>1.176283863655371</v>
       </c>
       <c r="AE24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.89027970953773305</v>
       </c>
       <c r="AF24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>1.3167310031726438</v>
       </c>
       <c r="AG24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.89606256911283799</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>7</v>
       </c>
       <c r="B25">
-        <f>FISHER(B9)</f>
+        <f t="shared" si="10"/>
         <v>1.1052111292293008</v>
       </c>
       <c r="C25">
-        <f>FISHER(C9)</f>
+        <f t="shared" si="10"/>
         <v>1.2676502479831251</v>
       </c>
       <c r="D25">
-        <f>FISHER(D9)</f>
+        <f t="shared" si="10"/>
         <v>0.43769274391033475</v>
       </c>
       <c r="E25">
-        <f>FISHER(E9)</f>
+        <f t="shared" si="10"/>
         <v>0.44907443265331198</v>
       </c>
       <c r="G25" s="1">
         <v>7</v>
       </c>
       <c r="H25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.95847827313738676</v>
       </c>
       <c r="I25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.0353685018639318</v>
       </c>
       <c r="J25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.33617483330716308</v>
       </c>
       <c r="K25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.72762062976238184</v>
       </c>
       <c r="M25" s="1">
         <v>7</v>
       </c>
       <c r="N25">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.52769758997265315</v>
       </c>
       <c r="O25">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.46075915773634329</v>
       </c>
       <c r="P25">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.14521190387399291</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.44628901520343256</v>
       </c>
       <c r="R25" s="1">
         <v>7</v>
       </c>
       <c r="S25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.327426996774685</v>
       </c>
       <c r="T25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.61285415003536159</v>
       </c>
       <c r="U25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.2997004881437058</v>
       </c>
       <c r="V25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.66392705888380399</v>
       </c>
       <c r="X25" s="1">
         <v>7</v>
       </c>
       <c r="Y25">
-        <f t="shared" ref="Y25:AB25" si="28">FISHER(Y9)</f>
+        <f t="shared" ref="Y25:AB25" si="29">FISHER(Y9)</f>
         <v>0.51998358286829927</v>
       </c>
       <c r="Z25">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.50649120355307731</v>
       </c>
       <c r="AA25">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.46749801263878693</v>
       </c>
       <c r="AB25">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.41756188581703185</v>
       </c>
       <c r="AC25" s="1">
         <v>7</v>
       </c>
       <c r="AD25">
-        <f t="shared" ref="AD25:AG25" si="29">FISHER(AD9)</f>
+        <f t="shared" ref="AD25:AG25" si="30">FISHER(AD9)</f>
         <v>1.3514991817161499</v>
       </c>
       <c r="AE25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.8643919771749401</v>
       </c>
       <c r="AF25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1.2867219817516937</v>
       </c>
       <c r="AG25">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0.76975314199711331</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>8</v>
       </c>
       <c r="B26">
-        <f>FISHER(B10)</f>
+        <f t="shared" si="10"/>
         <v>0.86176167995032926</v>
       </c>
       <c r="C26">
-        <f>FISHER(C10)</f>
+        <f t="shared" si="10"/>
         <v>1.0597806187509302</v>
       </c>
       <c r="D26">
-        <f>FISHER(D10)</f>
+        <f t="shared" si="10"/>
         <v>0.54632626588267974</v>
       </c>
       <c r="E26">
-        <f>FISHER(E10)</f>
+        <f t="shared" si="10"/>
         <v>0.4976239598783806</v>
       </c>
       <c r="G26" s="1">
         <v>8</v>
       </c>
       <c r="H26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.65303958265185358</v>
       </c>
       <c r="I26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.1218650647428672</v>
       </c>
       <c r="J26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.41490129601731596</v>
       </c>
       <c r="K26">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.70683448317988151</v>
       </c>
       <c r="M26" s="1">
         <v>8</v>
       </c>
       <c r="N26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.53076205452069714</v>
       </c>
       <c r="O26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.56753052081840172</v>
       </c>
       <c r="P26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.37299669544860931</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.76429804339118035</v>
       </c>
       <c r="R26" s="1">
         <v>8</v>
       </c>
       <c r="S26">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.4515736644883257</v>
       </c>
       <c r="T26">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.83423214232006282</v>
       </c>
       <c r="U26">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.82571130326269349</v>
       </c>
       <c r="V26">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.48367222966617729</v>
       </c>
       <c r="X26" s="1">
         <v>8</v>
       </c>
       <c r="Y26">
-        <f t="shared" ref="Y26:AB26" si="30">FISHER(Y10)</f>
+        <f t="shared" ref="Y26:AB26" si="31">FISHER(Y10)</f>
         <v>0.65357756080517315</v>
       </c>
       <c r="Z26">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.35602999100791183</v>
       </c>
       <c r="AA26">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.59814437786832786</v>
       </c>
       <c r="AB26">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0.48679914407995795</v>
       </c>
       <c r="AC26" s="1">
         <v>8</v>
       </c>
       <c r="AD26">
-        <f t="shared" ref="AD26:AG26" si="31">FISHER(AD10)</f>
+        <f t="shared" ref="AD26:AG26" si="32">FISHER(AD10)</f>
         <v>1.3071825171044591</v>
       </c>
       <c r="AE26">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.94472723430044014</v>
       </c>
       <c r="AF26">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.87417408447257738</v>
       </c>
       <c r="AG26">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.86873900877664312</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>9</v>
       </c>
       <c r="B27">
-        <f>FISHER(B11)</f>
+        <f t="shared" si="10"/>
         <v>1.2545346013248939</v>
       </c>
       <c r="C27">
-        <f>FISHER(C11)</f>
+        <f t="shared" si="10"/>
         <v>1.2365984232530338</v>
       </c>
       <c r="D27">
-        <f>FISHER(D11)</f>
+        <f t="shared" si="10"/>
         <v>0.96260660153007227</v>
       </c>
       <c r="E27">
-        <f>FISHER(E11)</f>
+        <f t="shared" si="10"/>
         <v>0.7643327138750835</v>
       </c>
       <c r="G27" s="1">
         <v>9</v>
       </c>
       <c r="H27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.0504907659830391</v>
       </c>
       <c r="I27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.96953922468943743</v>
       </c>
       <c r="J27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.85976287030191811</v>
       </c>
       <c r="K27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.74523612066751943</v>
       </c>
       <c r="M27" s="1">
         <v>9</v>
       </c>
       <c r="N27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.58081941420187477</v>
       </c>
       <c r="O27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.52828411476990478</v>
       </c>
       <c r="P27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.68218817933912179</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.80066036603631663</v>
       </c>
       <c r="R27" s="1">
         <v>9</v>
       </c>
       <c r="S27">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.0335076589653989</v>
       </c>
       <c r="T27">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.91175088977643637</v>
       </c>
       <c r="U27">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.2762024214131344</v>
       </c>
       <c r="V27">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.85271333634760815</v>
       </c>
       <c r="X27" s="1">
         <v>9</v>
       </c>
       <c r="Y27">
-        <f t="shared" ref="Y27:AB27" si="32">FISHER(Y11)</f>
+        <f t="shared" ref="Y27:AB27" si="33">FISHER(Y11)</f>
         <v>1.1180832592112073</v>
       </c>
       <c r="Z27">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>1.2100091616897284E-2</v>
       </c>
       <c r="AA27">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>1.2514550555107757</v>
       </c>
       <c r="AB27">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.43215368610237148</v>
       </c>
       <c r="AC27" s="1">
         <v>9</v>
       </c>
       <c r="AD27">
-        <f t="shared" ref="AD27:AG27" si="33">FISHER(AD11)</f>
+        <f t="shared" ref="AD27:AG27" si="34">FISHER(AD11)</f>
         <v>1.2801360851087122</v>
       </c>
       <c r="AE27">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>0.96518837796961299</v>
       </c>
       <c r="AF27">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1.3297712554564656</v>
       </c>
       <c r="AG27">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1.0084029327538395</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>10</v>
       </c>
       <c r="B28">
-        <f>FISHER(B12)</f>
+        <f t="shared" si="10"/>
         <v>1.1177489389945985</v>
       </c>
       <c r="C28">
-        <f>FISHER(C12)</f>
+        <f t="shared" si="10"/>
         <v>1.0880989577193874</v>
       </c>
       <c r="D28">
-        <f>FISHER(D12)</f>
+        <f t="shared" si="10"/>
         <v>0.44370145116310583</v>
       </c>
       <c r="E28">
-        <f>FISHER(E12)</f>
+        <f t="shared" si="10"/>
         <v>0.32345465580457033</v>
       </c>
       <c r="G28" s="1">
         <v>10</v>
       </c>
       <c r="H28">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.0216896817443288</v>
       </c>
       <c r="I28">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.0362238978568226</v>
       </c>
       <c r="J28">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.8030694359950622</v>
       </c>
       <c r="K28">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.79396661079812814</v>
       </c>
       <c r="M28" s="1">
         <v>10</v>
       </c>
       <c r="N28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.63022394931481973</v>
       </c>
       <c r="O28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.3660505600496563</v>
       </c>
       <c r="P28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.55404119541005459</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.73991050939709191</v>
       </c>
       <c r="R28" s="1">
         <v>10</v>
       </c>
       <c r="S28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.2310669249768762</v>
       </c>
       <c r="T28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.6949272690893904</v>
       </c>
       <c r="U28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.2753557283411874</v>
       </c>
       <c r="V28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.76747016338807827</v>
       </c>
       <c r="X28" s="1">
         <v>10</v>
       </c>
       <c r="Y28">
-        <f t="shared" ref="Y28:AB28" si="34">FISHER(Y12)</f>
+        <f t="shared" ref="Y28:AB28" si="35">FISHER(Y12)</f>
         <v>0.46810337678378033</v>
       </c>
       <c r="Z28">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>-6.3814944966139389E-2</v>
       </c>
       <c r="AA28">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>0.6355081674018771</v>
       </c>
       <c r="AB28">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>9.9193468757480779E-2</v>
       </c>
       <c r="AC28" s="1">
         <v>10</v>
       </c>
       <c r="AD28">
-        <f t="shared" ref="AD28:AG28" si="35">FISHER(AD12)</f>
+        <f t="shared" ref="AD28:AG28" si="36">FISHER(AD12)</f>
         <v>1.3005752876475176</v>
       </c>
       <c r="AE28">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.49891684889764465</v>
       </c>
       <c r="AF28">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>1.3476191676198106</v>
       </c>
       <c r="AG28">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0.71737678888944567</v>
       </c>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>11</v>
       </c>
       <c r="B29">
-        <f>FISHER(B13)</f>
+        <f t="shared" si="10"/>
         <v>1.2656821178024134</v>
       </c>
       <c r="C29">
-        <f>FISHER(C13)</f>
+        <f t="shared" si="10"/>
         <v>1.2876159351021996</v>
       </c>
       <c r="D29">
-        <f>FISHER(D13)</f>
+        <f t="shared" si="10"/>
         <v>0.60594433766114719</v>
       </c>
       <c r="E29">
-        <f>FISHER(E13)</f>
+        <f t="shared" si="10"/>
         <v>0.64018213197416785</v>
       </c>
       <c r="G29" s="1">
         <v>11</v>
       </c>
       <c r="H29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.73623909885489924</v>
       </c>
       <c r="I29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.97806616031714555</v>
       </c>
       <c r="J29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.48199200944345855</v>
       </c>
       <c r="K29">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.69488555320996648</v>
       </c>
       <c r="M29" s="1">
         <v>11</v>
       </c>
       <c r="N29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.67791581939742573</v>
       </c>
       <c r="O29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.20006732373624897</v>
       </c>
       <c r="P29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.43799545277323959</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.1735058353564832</v>
       </c>
       <c r="R29" s="1">
         <v>11</v>
       </c>
       <c r="S29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.4157427549014336</v>
       </c>
       <c r="T29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.92360165618710111</v>
       </c>
       <c r="U29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.0289843250033779</v>
       </c>
       <c r="V29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.83138491026327632</v>
       </c>
       <c r="X29" s="1">
         <v>11</v>
       </c>
       <c r="Y29">
-        <f t="shared" ref="Y29:AB29" si="36">FISHER(Y13)</f>
+        <f t="shared" ref="Y29:AB29" si="37">FISHER(Y13)</f>
         <v>0.75297104540696669</v>
       </c>
       <c r="Z29">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0.47883786645421073</v>
       </c>
       <c r="AA29">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0.70883353207022071</v>
       </c>
       <c r="AB29">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0.30110637683534125</v>
       </c>
       <c r="AC29" s="1">
         <v>11</v>
       </c>
       <c r="AD29">
-        <f t="shared" ref="AD29:AG29" si="37">FISHER(AD13)</f>
+        <f t="shared" ref="AD29:AG29" si="38">FISHER(AD13)</f>
         <v>1.5238373790410964</v>
       </c>
       <c r="AE29">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0.97163389326752736</v>
       </c>
       <c r="AF29">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>1.4319889806803172</v>
       </c>
       <c r="AG29">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>1.0451106670378081</v>
       </c>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>12</v>
       </c>
       <c r="B30">
-        <f>FISHER(B14)</f>
+        <f t="shared" si="10"/>
         <v>1.2866579124310105</v>
       </c>
       <c r="C30">
-        <f>FISHER(C14)</f>
+        <f t="shared" si="10"/>
         <v>1.1869659725317423</v>
       </c>
       <c r="D30">
-        <f>FISHER(D14)</f>
+        <f t="shared" si="10"/>
         <v>0.66421666180337469</v>
       </c>
       <c r="E30">
-        <f>FISHER(E14)</f>
+        <f t="shared" si="10"/>
         <v>0.61539667067733661</v>
       </c>
       <c r="G30" s="1">
         <v>12</v>
       </c>
       <c r="H30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.3907563606915261</v>
       </c>
       <c r="I30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.3895013800909604</v>
       </c>
       <c r="J30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.0504320823765825</v>
       </c>
       <c r="K30">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.1139977962783232</v>
       </c>
       <c r="M30" s="1">
         <v>12</v>
       </c>
       <c r="N30">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.9081794986668642</v>
       </c>
       <c r="O30">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.94244718415088324</v>
       </c>
       <c r="P30">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.78620620364683935</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.0798426065239799</v>
       </c>
       <c r="R30" s="1">
         <v>12</v>
       </c>
       <c r="S30">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.5333168428418149</v>
       </c>
       <c r="T30">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.251499945331338</v>
       </c>
       <c r="U30">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.7219599618696968</v>
       </c>
       <c r="V30">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.1173716815579187</v>
       </c>
       <c r="X30" s="1">
         <v>12</v>
       </c>
       <c r="Y30">
-        <f t="shared" ref="Y30:AB30" si="38">FISHER(Y14)</f>
+        <f t="shared" ref="Y30:AB30" si="39">FISHER(Y14)</f>
         <v>0.81582471504002774</v>
       </c>
       <c r="Z30">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.3231902010461043</v>
       </c>
       <c r="AA30">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.67904822835374523</v>
       </c>
       <c r="AB30">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0.80330837120212439</v>
       </c>
       <c r="AC30" s="1">
         <v>12</v>
       </c>
       <c r="AD30">
-        <f t="shared" ref="AD30:AG30" si="39">FISHER(AD14)</f>
+        <f t="shared" ref="AD30:AG30" si="40">FISHER(AD14)</f>
         <v>1.2936537962449164</v>
       </c>
       <c r="AE30">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.70932355371686884</v>
       </c>
       <c r="AF30">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1.4682688066404106</v>
       </c>
       <c r="AG30">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0.84668519452880531</v>
       </c>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
@@ -3340,15 +3383,15 @@
         <v>1.1027508229174476</v>
       </c>
       <c r="C31">
-        <f t="shared" ref="C31:E31" si="40">AVERAGE(C19:C30)</f>
+        <f t="shared" ref="C31:E31" si="41">AVERAGE(C19:C30)</f>
         <v>1.1236397719247619</v>
       </c>
       <c r="D31">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>0.70783082489573879</v>
       </c>
       <c r="E31">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>0.54840608193615714</v>
       </c>
       <c r="G31" s="1" t="s">
@@ -3359,15 +3402,15 @@
         <v>0.9634309130246651</v>
       </c>
       <c r="I31">
-        <f t="shared" ref="I31:K31" si="41">AVERAGE(I19:I30)</f>
+        <f t="shared" ref="I31:K31" si="42">AVERAGE(I19:I30)</f>
         <v>1.0348766686692219</v>
       </c>
       <c r="J31">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>0.70267411632043297</v>
       </c>
       <c r="K31">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>0.72981202628713848</v>
       </c>
       <c r="M31" s="1" t="s">
@@ -3378,15 +3421,15 @@
         <v>0.65431007044898593</v>
       </c>
       <c r="O31">
-        <f t="shared" ref="O31:Q31" si="42">AVERAGE(O19:O30)</f>
+        <f t="shared" ref="O31:Q31" si="43">AVERAGE(O19:O30)</f>
         <v>0.54718052424031849</v>
       </c>
       <c r="P31">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>0.61523988859365975</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>0.66930588218414944</v>
       </c>
       <c r="R31" s="1" t="s">
@@ -3397,15 +3440,15 @@
         <v>1.2734814048054768</v>
       </c>
       <c r="T31">
-        <f t="shared" ref="T31:V31" si="43">AVERAGE(T19:T30)</f>
+        <f t="shared" ref="T31:V31" si="44">AVERAGE(T19:T30)</f>
         <v>0.79773090931181301</v>
       </c>
       <c r="U31">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>1.2341260302260559</v>
       </c>
       <c r="V31">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>0.76603039063270162</v>
       </c>
       <c r="X31" s="1" t="s">
@@ -3416,15 +3459,15 @@
         <v>0.70534592106752614</v>
       </c>
       <c r="Z31">
-        <f t="shared" ref="Z31" si="44">AVERAGE(Z19:Z30)</f>
+        <f t="shared" ref="Z31" si="45">AVERAGE(Z19:Z30)</f>
         <v>0.31687842523732113</v>
       </c>
       <c r="AA31">
-        <f t="shared" ref="AA31" si="45">AVERAGE(AA19:AA30)</f>
+        <f t="shared" ref="AA31" si="46">AVERAGE(AA19:AA30)</f>
         <v>0.81696078454181442</v>
       </c>
       <c r="AB31">
-        <f t="shared" ref="AB31" si="46">AVERAGE(AB19:AB30)</f>
+        <f t="shared" ref="AB31" si="47">AVERAGE(AB19:AB30)</f>
         <v>0.51746037598815464</v>
       </c>
       <c r="AC31" s="1" t="s">
@@ -3435,32 +3478,619 @@
         <v>1.2831650891645179</v>
       </c>
       <c r="AE31">
-        <f t="shared" ref="AE31" si="47">AVERAGE(AE19:AE30)</f>
+        <f t="shared" ref="AE31" si="48">AVERAGE(AE19:AE30)</f>
         <v>0.7600182179327305</v>
       </c>
       <c r="AF31">
-        <f t="shared" ref="AF31" si="48">AVERAGE(AF19:AF30)</f>
+        <f t="shared" ref="AF31" si="49">AVERAGE(AF19:AF30)</f>
         <v>1.3015525656288134</v>
       </c>
       <c r="AG31">
-        <f t="shared" ref="AG31" si="49">AVERAGE(AG19:AG30)</f>
+        <f t="shared" ref="AG31" si="50">AVERAGE(AG19:AG30)</f>
         <v>0.79036589705353422</v>
       </c>
     </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="H33" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H34" t="s">
+        <v>27</v>
+      </c>
+      <c r="I34" t="s">
+        <v>28</v>
+      </c>
+      <c r="J34" t="s">
+        <v>29</v>
+      </c>
+      <c r="K34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>0.75347499834384202</v>
+      </c>
+      <c r="C35">
+        <v>0.55016103738813205</v>
+      </c>
+      <c r="D35">
+        <v>0.74048651161782697</v>
+      </c>
+      <c r="E35">
+        <v>0.49826687702246297</v>
+      </c>
+      <c r="G35" s="2">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <f>FISHER(B35)</f>
+        <v>0.9809456981989032</v>
+      </c>
+      <c r="I35">
+        <f t="shared" ref="I35:K46" si="51">FISHER(C35)</f>
+        <v>0.61861222087565892</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="51"/>
+        <v>0.95155563894908002</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="51"/>
+        <v>0.54699797648607218</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>2</v>
+      </c>
+      <c r="B36">
+        <v>0.79655299851851002</v>
+      </c>
+      <c r="C36">
+        <v>0.56865570573520896</v>
+      </c>
+      <c r="D36">
+        <v>0.84370238532753605</v>
+      </c>
+      <c r="E36">
+        <v>0.183954519429326</v>
+      </c>
+      <c r="G36" s="2">
+        <v>2</v>
+      </c>
+      <c r="H36">
+        <f t="shared" ref="H36:H46" si="52">FISHER(B36)</f>
+        <v>1.0891097855598351</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="51"/>
+        <v>0.64553384768181499</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="51"/>
+        <v>1.2338845093746138</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="51"/>
+        <v>0.18607265632881434</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <v>0.753901416032842</v>
+      </c>
+      <c r="C37">
+        <v>0.64430991910325597</v>
+      </c>
+      <c r="D37">
+        <v>0.74195178308472898</v>
+      </c>
+      <c r="E37">
+        <v>0.488969711666984</v>
+      </c>
+      <c r="G37" s="2">
+        <v>3</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="52"/>
+        <v>0.98193288131887679</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="51"/>
+        <v>0.76550814035127535</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="51"/>
+        <v>0.95480751162233868</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="51"/>
+        <v>0.53470541498520008</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>0.45752358134919502</v>
+      </c>
+      <c r="C38">
+        <v>0.22507625491345501</v>
+      </c>
+      <c r="D38">
+        <v>0.67982233262576797</v>
+      </c>
+      <c r="E38">
+        <v>0.42248850377512698</v>
+      </c>
+      <c r="G38" s="2">
+        <v>4</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="52"/>
+        <v>0.49417474043101584</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="51"/>
+        <v>0.22899686943735412</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="51"/>
+        <v>0.82878363007479616</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="51"/>
+        <v>0.45071736759123326</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>0.65738620878374998</v>
+      </c>
+      <c r="C39">
+        <v>0.53378225036382598</v>
+      </c>
+      <c r="D39">
+        <v>0.68786661838637597</v>
+      </c>
+      <c r="E39">
+        <v>0.58101820669267101</v>
+      </c>
+      <c r="G39" s="2">
+        <v>5</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="52"/>
+        <v>0.78819661386717965</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="51"/>
+        <v>0.59541961202578431</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="51"/>
+        <v>0.84389502643159109</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="51"/>
+        <v>0.6639984434134526</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>6</v>
+      </c>
+      <c r="B40">
+        <v>0.726185974499167</v>
+      </c>
+      <c r="C40">
+        <v>0.57397211989062802</v>
+      </c>
+      <c r="D40">
+        <v>0.77221990840304</v>
+      </c>
+      <c r="E40">
+        <v>0.295406058020519</v>
+      </c>
+      <c r="G40" s="2">
+        <v>6</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="52"/>
+        <v>0.92061023889363325</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="51"/>
+        <v>0.65342646276172656</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="51"/>
+        <v>1.0258037861487113</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="51"/>
+        <v>0.30447890762321467</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>7</v>
+      </c>
+      <c r="B41">
+        <v>0.71132921476546296</v>
+      </c>
+      <c r="C41">
+        <v>0.26742321649434397</v>
+      </c>
+      <c r="D41">
+        <v>0.75874366170836205</v>
+      </c>
+      <c r="E41">
+        <v>0.41987771070191199</v>
+      </c>
+      <c r="G41" s="2">
+        <v>7</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="52"/>
+        <v>0.88986938938435212</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="51"/>
+        <v>0.27408649781579969</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="51"/>
+        <v>0.99324749598752538</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="51"/>
+        <v>0.4475435513646806</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>8</v>
+      </c>
+      <c r="B42">
+        <v>0.71031066815787103</v>
+      </c>
+      <c r="C42">
+        <v>0.49484546354319903</v>
+      </c>
+      <c r="D42">
+        <v>0.68282241667703802</v>
+      </c>
+      <c r="E42">
+        <v>0.39012155154561101</v>
+      </c>
+      <c r="G42" s="2">
+        <v>8</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="52"/>
+        <v>0.88781061551469242</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="51"/>
+        <v>0.54245685818284506</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="51"/>
+        <v>0.83438292795253388</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="51"/>
+        <v>0.41194339848698053</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>9</v>
+      </c>
+      <c r="B43">
+        <v>0.75822280448342305</v>
+      </c>
+      <c r="C43">
+        <v>0.485897736166713</v>
+      </c>
+      <c r="D43">
+        <v>0.77879628975647996</v>
+      </c>
+      <c r="E43">
+        <v>0.480904991878849</v>
+      </c>
+      <c r="G43" s="2">
+        <v>9</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="52"/>
+        <v>0.99202109265184724</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="51"/>
+        <v>0.53067610108883523</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="51"/>
+        <v>1.0423040650307074</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="51"/>
+        <v>0.52416086725145739</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>10</v>
+      </c>
+      <c r="B44">
+        <v>0.75828235477871497</v>
+      </c>
+      <c r="C44">
+        <v>0.35157369554888601</v>
+      </c>
+      <c r="D44">
+        <v>0.69926901214468595</v>
+      </c>
+      <c r="E44">
+        <v>0.278120915371524</v>
+      </c>
+      <c r="G44" s="2">
+        <v>10</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="52"/>
+        <v>0.99216119351453314</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="51"/>
+        <v>0.36723826782630176</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="51"/>
+        <v>0.86586865381719758</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="51"/>
+        <v>0.28564429568738797</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>11</v>
+      </c>
+      <c r="B45">
+        <v>0.604518823295353</v>
+      </c>
+      <c r="C45">
+        <v>0.276144970659642</v>
+      </c>
+      <c r="D45">
+        <v>0.80102401564164505</v>
+      </c>
+      <c r="E45">
+        <v>0.41630587919610601</v>
+      </c>
+      <c r="G45" s="2">
+        <v>11</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="52"/>
+        <v>0.70023799981885571</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="51"/>
+        <v>0.28350396710135972</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="51"/>
+        <v>1.1014632719382471</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="51"/>
+        <v>0.44321509371931966</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>12</v>
+      </c>
+      <c r="B46">
+        <v>0.810394502092459</v>
+      </c>
+      <c r="C46">
+        <v>0.55903109636888804</v>
+      </c>
+      <c r="D46">
+        <v>0.80038065410860704</v>
+      </c>
+      <c r="E46">
+        <v>0.64605119224457797</v>
+      </c>
+      <c r="G46" s="2">
+        <v>12</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="52"/>
+        <v>1.1281772353323585</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="51"/>
+        <v>0.63142272778112329</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="51"/>
+        <v>1.0996705567736405</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="51"/>
+        <v>0.76849109496814949</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47">
+        <f>AVERAGE(B35:B46)</f>
+        <v>0.70817362875838263</v>
+      </c>
+      <c r="C47">
+        <f t="shared" ref="C47:E47" si="53">AVERAGE(C35:C46)</f>
+        <v>0.46090612218134819</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="53"/>
+        <v>0.74892379912350782</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="53"/>
+        <v>0.42512384312880586</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H47">
+        <f>AVERAGE(H35:H46)</f>
+        <v>0.90377062370717365</v>
+      </c>
+      <c r="I47">
+        <f t="shared" ref="I47:K47" si="54">AVERAGE(I35:I46)</f>
+        <v>0.51140679774415665</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="54"/>
+        <v>0.98130558950841518</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="54"/>
+        <v>0.46399742232549696</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="G52" s="2"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="G53" s="2"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+      <c r="G54" s="2"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+      <c r="G55" s="2"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="G56" s="2"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+      <c r="G57" s="2"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+      <c r="G59" s="2"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="G60" s="2"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+      <c r="G61" s="2"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="G62" s="2"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="G63" s="2"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+      <c r="G64" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="N17:Q17"/>
     <mergeCell ref="S1:V1"/>
     <mergeCell ref="S17:V17"/>
     <mergeCell ref="Y1:AB1"/>
     <mergeCell ref="AD1:AG1"/>
     <mergeCell ref="Y17:AB17"/>
     <mergeCell ref="AD17:AG17"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="H17:K17"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="N17:Q17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>